<commit_message>
Filter and Summarization Patterns added.
</commit_message>
<xml_diff>
--- a/Hadoop.xlsx
+++ b/Hadoop.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\ML\Hadoop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Desktop\ML\Hadoop\udacity_intro_to_hadoop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6A2AB0-B86A-472A-ADEA-4FDD1B42C04E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8016D830-502E-49C9-B133-AF657C946F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F841DBE3-804C-4506-8165-0EAA69F1CBAE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F841DBE3-804C-4506-8165-0EAA69F1CBAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hadoop Ecosystem" sheetId="1" r:id="rId1"/>
     <sheet name="HDFS" sheetId="3" r:id="rId2"/>
     <sheet name="MapReduce" sheetId="4" r:id="rId3"/>
+    <sheet name="Design Pattern" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>The 3 Vs</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>The Daemon that splits the work into Mappers and Reducers</t>
+  </si>
+  <si>
+    <t>Filtering Patterns</t>
+  </si>
+  <si>
+    <t>Summarization Patterns</t>
+  </si>
+  <si>
+    <t>Structural Patterns</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE3D6D7-3ADD-4683-AFAA-7FB88BF4D143}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1558,4 +1567,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ABB3D3-CCD8-4133-8E2B-D1E39CEC825B}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>